<commit_message>
merged last commit some changes still left
</commit_message>
<xml_diff>
--- a/MAU.xlsx
+++ b/MAU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15s\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE751C8-40FB-40FD-8E80-530ABA21052F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC64CF2D-E38D-4AD8-AC10-4201748D4F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>ADDITIONAL_CHARGES</t>
   </si>
   <si>
-    <t>DESCRIPTION</t>
-  </si>
-  <si>
     <t>ADD_ONS</t>
   </si>
   <si>
@@ -226,9 +223,6 @@
     <t>107678785433655</t>
   </si>
   <si>
-    <t>Null</t>
-  </si>
-  <si>
     <t>Delcart</t>
   </si>
   <si>
@@ -740,6 +734,12 @@
   </si>
   <si>
     <t>Aug</t>
+  </si>
+  <si>
+    <t>DESCRIP</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -1088,8 +1088,8 @@
   </sheetPr>
   <dimension ref="A1:AA987"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J38" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1142,13 +1142,13 @@
         <v>12</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
@@ -1164,50 +1164,50 @@
     </row>
     <row r="2" spans="1:27" ht="14.25" customHeight="1">
       <c r="A2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="G2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J2" s="6">
         <v>6569</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="N2" s="4"/>
       <c r="O2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
@@ -1223,50 +1223,50 @@
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1">
       <c r="A3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="G3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J3" s="7">
         <v>591</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
@@ -1282,50 +1282,50 @@
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="I4" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
@@ -1341,50 +1341,50 @@
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="C5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
@@ -1400,52 +1400,52 @@
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
@@ -1461,50 +1461,50 @@
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q7" s="4"/>
       <c r="R7" s="4"/>
@@ -1520,52 +1520,52 @@
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
       <c r="A8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L8" s="4" t="s">
+      <c r="M8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N8" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="O8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
@@ -1581,52 +1581,52 @@
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1">
       <c r="A9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q9" s="4"/>
       <c r="R9" s="4"/>
@@ -1642,50 +1642,50 @@
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1">
       <c r="A10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="R10" s="4"/>
@@ -1701,52 +1701,52 @@
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="5" t="s">
+      <c r="G11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="O11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="4"/>
       <c r="R11" s="4"/>
@@ -1762,52 +1762,52 @@
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1">
       <c r="A12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N12" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="O12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
@@ -1823,50 +1823,50 @@
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1">
       <c r="A13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>67</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I13" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="M13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q13" s="4"/>
       <c r="R13" s="4"/>
@@ -1882,50 +1882,50 @@
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1">
       <c r="A14" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M14" s="4" t="s">
-        <v>71</v>
       </c>
       <c r="N14" s="4"/>
       <c r="O14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
@@ -1941,50 +1941,50 @@
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="G15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="I15" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
@@ -2000,50 +2000,50 @@
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
@@ -2059,50 +2059,50 @@
     </row>
     <row r="17" spans="1:27" ht="14.25" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="F17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="M17" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N17" s="4"/>
       <c r="O17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
@@ -2118,50 +2118,50 @@
     </row>
     <row r="18" spans="1:27" ht="14.25" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q18" s="4"/>
       <c r="R18" s="4"/>
@@ -2177,50 +2177,50 @@
     </row>
     <row r="19" spans="1:27" ht="14.25" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q19" s="4"/>
       <c r="R19" s="4"/>
@@ -2236,50 +2236,50 @@
     </row>
     <row r="20" spans="1:27" ht="14.25" customHeight="1">
       <c r="A20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="E20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="G20" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
@@ -2295,50 +2295,50 @@
     </row>
     <row r="21" spans="1:27" ht="14.25" customHeight="1">
       <c r="A21" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
@@ -2354,52 +2354,52 @@
     </row>
     <row r="22" spans="1:27" ht="14.25" customHeight="1">
       <c r="A22" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P22" s="4" t="s">
         <v>93</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O22" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="P22" s="4" t="s">
-        <v>95</v>
       </c>
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
@@ -2415,50 +2415,50 @@
     </row>
     <row r="23" spans="1:27" ht="14.25" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N23" s="4"/>
       <c r="O23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
@@ -2474,50 +2474,50 @@
     </row>
     <row r="24" spans="1:27" ht="14.25" customHeight="1">
       <c r="A24" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
@@ -2533,50 +2533,50 @@
     </row>
     <row r="25" spans="1:27" ht="14.25" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N25" s="4"/>
       <c r="O25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q25" s="4"/>
       <c r="R25" s="4"/>
@@ -2592,50 +2592,50 @@
     </row>
     <row r="26" spans="1:27" ht="14.25" customHeight="1">
       <c r="A26" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N26" s="4"/>
       <c r="O26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
@@ -2651,50 +2651,50 @@
     </row>
     <row r="27" spans="1:27" ht="14.25" customHeight="1">
       <c r="A27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="D27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J27" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N27" s="4"/>
       <c r="O27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q27" s="4"/>
       <c r="R27" s="4"/>
@@ -2710,50 +2710,50 @@
     </row>
     <row r="28" spans="1:27" ht="14.25" customHeight="1">
       <c r="A28" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>29</v>
-      </c>
       <c r="E28" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J28" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N28" s="4"/>
       <c r="O28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
@@ -2769,50 +2769,50 @@
     </row>
     <row r="29" spans="1:27" ht="14.25" customHeight="1">
       <c r="A29" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="G29" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J29" s="8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
@@ -2828,50 +2828,50 @@
     </row>
     <row r="30" spans="1:27" ht="14.25" customHeight="1">
       <c r="A30" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="E30" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N30" s="4"/>
       <c r="O30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q30" s="4"/>
       <c r="R30" s="4"/>
@@ -2887,50 +2887,50 @@
     </row>
     <row r="31" spans="1:27" ht="14.25" customHeight="1">
       <c r="A31" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D31" s="11" t="s">
+      <c r="E31" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J31" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="K31" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N31" s="4"/>
       <c r="O31" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q31" s="4"/>
       <c r="R31" s="4"/>
@@ -2946,50 +2946,50 @@
     </row>
     <row r="32" spans="1:27" ht="14.25" customHeight="1">
       <c r="A32" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="I32" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N32" s="4"/>
       <c r="O32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q32" s="4"/>
       <c r="R32" s="4"/>
@@ -3005,50 +3005,50 @@
     </row>
     <row r="33" spans="1:27" ht="14.25" customHeight="1">
       <c r="A33" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J33" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N33" s="4"/>
       <c r="O33" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P33" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="Q33" s="4"/>
       <c r="R33" s="4"/>
@@ -3064,52 +3064,52 @@
     </row>
     <row r="34" spans="1:27" ht="14.25" customHeight="1">
       <c r="A34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L34" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="M34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="N34" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J34" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L34" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="M34" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="N34" s="4" t="s">
-        <v>129</v>
-      </c>
       <c r="O34" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P34" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q34" s="4"/>
       <c r="R34" s="4"/>
@@ -3125,50 +3125,50 @@
     </row>
     <row r="35" spans="1:27" ht="14.25" customHeight="1">
       <c r="A35" s="5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J35" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K35" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N35" s="4"/>
       <c r="O35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q35" s="4"/>
       <c r="R35" s="4"/>
@@ -3184,50 +3184,50 @@
     </row>
     <row r="36" spans="1:27" ht="14.25" customHeight="1">
       <c r="A36" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="E36" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N36" s="4"/>
       <c r="O36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q36" s="4"/>
       <c r="R36" s="4"/>
@@ -3243,50 +3243,50 @@
     </row>
     <row r="37" spans="1:27" ht="14.25" customHeight="1">
       <c r="A37" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H37" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J37" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N37" s="4"/>
       <c r="O37" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P37" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q37" s="4"/>
       <c r="R37" s="4"/>
@@ -3302,50 +3302,50 @@
     </row>
     <row r="38" spans="1:27" ht="14.25" customHeight="1">
       <c r="A38" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="D38" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="E38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="I38" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M38" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="N38" s="4"/>
       <c r="O38" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P38" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q38" s="4"/>
       <c r="R38" s="4"/>
@@ -3361,52 +3361,52 @@
     </row>
     <row r="39" spans="1:27" ht="14.25" customHeight="1">
       <c r="A39" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G39" s="5" t="s">
+      <c r="I39" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H39" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J39" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="N39" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="O39" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P39" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q39" s="4"/>
       <c r="R39" s="4"/>
@@ -3422,50 +3422,50 @@
     </row>
     <row r="40" spans="1:27" ht="14.25" customHeight="1">
       <c r="A40" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J40" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M40" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="N40" s="4"/>
       <c r="O40" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P40" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
@@ -3481,50 +3481,50 @@
     </row>
     <row r="41" spans="1:27" ht="14.25" customHeight="1">
       <c r="A41" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="E41" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="F41" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E41" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>156</v>
-      </c>
       <c r="G41" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J41" s="8" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K41" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N41" s="4"/>
       <c r="O41" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P41" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q41" s="4"/>
       <c r="R41" s="4"/>
@@ -3540,50 +3540,50 @@
     </row>
     <row r="42" spans="1:27" ht="14.25" customHeight="1">
       <c r="A42" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>159</v>
-      </c>
       <c r="D42" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H42" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N42" s="4"/>
       <c r="O42" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P42" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q42" s="4"/>
       <c r="R42" s="4"/>
@@ -3599,50 +3599,50 @@
     </row>
     <row r="43" spans="1:27" ht="14.25" customHeight="1">
       <c r="A43" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J43" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N43" s="4"/>
       <c r="O43" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P43" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -3658,50 +3658,50 @@
     </row>
     <row r="44" spans="1:27" ht="14.25" customHeight="1">
       <c r="A44" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>166</v>
-      </c>
       <c r="F44" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="N44" s="4"/>
       <c r="O44" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P44" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
@@ -3717,50 +3717,50 @@
     </row>
     <row r="45" spans="1:27" ht="14.25" customHeight="1">
       <c r="A45" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>169</v>
-      </c>
       <c r="D45" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H45" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N45" s="4"/>
       <c r="O45" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P45" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
@@ -3776,50 +3776,50 @@
     </row>
     <row r="46" spans="1:27" ht="14.25" customHeight="1">
       <c r="A46" s="14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N46" s="4"/>
       <c r="O46" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P46" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
@@ -3835,50 +3835,50 @@
     </row>
     <row r="47" spans="1:27" ht="14.25" customHeight="1">
       <c r="A47" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="L47" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I47" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="J47" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="M47" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N47" s="4"/>
       <c r="O47" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P47" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q47" s="4"/>
       <c r="R47" s="4"/>
@@ -3894,50 +3894,50 @@
     </row>
     <row r="48" spans="1:27" ht="14.25" customHeight="1">
       <c r="A48" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J48" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N48" s="4"/>
       <c r="O48" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P48" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
@@ -3953,50 +3953,50 @@
     </row>
     <row r="49" spans="1:27" ht="14.25" customHeight="1">
       <c r="A49" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J49" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N49" s="4"/>
       <c r="O49" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P49" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
@@ -4012,50 +4012,50 @@
     </row>
     <row r="50" spans="1:27" ht="14.25" customHeight="1">
       <c r="A50" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J50" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N50" s="4"/>
       <c r="O50" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P50" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
@@ -4071,50 +4071,50 @@
     </row>
     <row r="51" spans="1:27" ht="14.25" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J51" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M51" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="M51" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="N51" s="4"/>
       <c r="O51" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P51" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q51" s="4"/>
       <c r="R51" s="4"/>
@@ -4130,50 +4130,50 @@
     </row>
     <row r="52" spans="1:27" ht="14.25" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J52" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M52" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="M52" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="N52" s="4"/>
       <c r="O52" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P52" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
@@ -4189,50 +4189,50 @@
     </row>
     <row r="53" spans="1:27" ht="14.25" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C53" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D53" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="E53" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J53" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N53" s="4"/>
       <c r="O53" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P53" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
@@ -4248,50 +4248,50 @@
     </row>
     <row r="54" spans="1:27" ht="14.25" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J54" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L54" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M54" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="M54" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="N54" s="4"/>
       <c r="O54" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P54" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q54" s="4"/>
       <c r="R54" s="4"/>
@@ -4307,50 +4307,50 @@
     </row>
     <row r="55" spans="1:27" ht="14.25" customHeight="1">
       <c r="A55" s="14" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C55" s="15">
         <v>30000</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J55" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="K55" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="K55" s="4" t="s">
-        <v>238</v>
-      </c>
       <c r="L55" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N55" s="4"/>
       <c r="O55" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P55" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q55" s="4"/>
       <c r="R55" s="4"/>
@@ -4366,50 +4366,50 @@
     </row>
     <row r="56" spans="1:27" ht="14.25" customHeight="1">
       <c r="A56" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C56" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="E56" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="F56" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J56" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N56" s="4"/>
       <c r="O56" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P56" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q56" s="4"/>
       <c r="R56" s="4"/>
@@ -4481,7 +4481,7 @@
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
       <c r="P63" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="64" spans="1:27" ht="14.4">

</xml_diff>